<commit_message>
new central campus data with rockefeller
</commit_message>
<xml_diff>
--- a/GPS Data Central.xlsx
+++ b/GPS Data Central.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Building</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Uris Library</t>
+  </si>
+  <si>
+    <t>Rockefeller Hall</t>
   </si>
 </sst>
 </file>
@@ -474,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="E18" sqref="C17:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -602,7 +605,7 @@
         <v>-76.485395506024304</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H17" si="0">SQRT((F3-D3)^2+(G3-E3)^2)/2</f>
+        <f t="shared" ref="H3:H16" si="0">SQRT((F3-D3)^2+(G3-E3)^2)/2</f>
         <v>3.3766958690000551E-4</v>
       </c>
       <c r="I3">
@@ -618,11 +621,11 @@
         <v>-76.4859004318714</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M18" si="1">SQRT((K3-I3)^2+(L3-J3)^2)/2</f>
+        <f t="shared" ref="M3:M19" si="1">SQRT((K3-I3)^2+(L3-J3)^2)/2</f>
         <v>3.9514574601643852E-4</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N18" si="2">AVERAGE(H3,M3)</f>
+        <f t="shared" ref="N3:N19" si="2">AVERAGE(H3,M3)</f>
         <v>3.6640766645822201E-4</v>
       </c>
     </row>
@@ -1329,6 +1332,53 @@
       <c r="N18">
         <f t="shared" si="2"/>
         <v>3.1150519269495803E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19">
+        <v>42.449079764950703</v>
+      </c>
+      <c r="C19">
+        <v>-76.481934785842896</v>
+      </c>
+      <c r="D19">
+        <v>42.448739351674803</v>
+      </c>
+      <c r="E19">
+        <v>-76.482149362564002</v>
+      </c>
+      <c r="F19">
+        <v>42.449459758980502</v>
+      </c>
+      <c r="G19">
+        <v>-76.481623649597097</v>
+      </c>
+      <c r="H19">
+        <f>SQRT((F19-D19)^2+(G19-E19)^2)/2</f>
+        <v>4.4591501703722392E-4</v>
+      </c>
+      <c r="I19">
+        <v>42.449428092899403</v>
+      </c>
+      <c r="J19">
+        <v>-76.482160091400104</v>
+      </c>
+      <c r="K19">
+        <v>42.448755184891397</v>
+      </c>
+      <c r="L19">
+        <v>-76.481537818908606</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="1"/>
+        <v>4.5826527277163288E-4</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="2"/>
+        <v>4.520901449044284E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>